<commit_message>
Signed-off-by: Leonardo Medeiros <Leonardo Medeiros>
</commit_message>
<xml_diff>
--- a/gqm/gqm2-tese-30.xlsx
+++ b/gqm/gqm2-tese-30.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -3692,9 +3692,9 @@
   </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3763,7 +3763,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -4141,7 +4141,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>20</v>
@@ -4179,7 +4179,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>20</v>
@@ -4875,7 +4875,7 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D32" s="11">
         <f>COUNTIF(D2:D31,"Sim")/COUNTA(D2:D31)</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="F32" s="11">
         <f t="shared" ref="F32:K32" si="0">COUNTIF(F2:F31,"Sim")/COUNTA(F2:F31)</f>
@@ -5492,7 +5492,7 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>